<commit_message>
Added dropdown to nav bar.
</commit_message>
<xml_diff>
--- a/People spreadsheet.xlsx
+++ b/People spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerrit\Documents\College BAAAAAYBEEEEEE\Math Bio Site\hymanlab.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BC3E66-0509-434C-A527-B6C0E43E4C37}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4931DF18-4975-4ACA-BE2E-EF0D4ECA697F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="5955" xr2:uid="{9C06E373-AECE-4E5B-9F33-8D3B6D0334FB}"/>
   </bookViews>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC129DD4-5708-4C25-BE56-42085CE9C315}">
   <dimension ref="B1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C2:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Zhe to spreadsheet.
</commit_message>
<xml_diff>
--- a/People spreadsheet.xlsx
+++ b/People spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerrit\Documents\College BAAAAAYBEEEEEE\Math Bio Site\hymanlab.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4931DF18-4975-4ACA-BE2E-EF0D4ECA697F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1178E035-1D47-4868-A81C-F535494F6803}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="5955" xr2:uid="{9C06E373-AECE-4E5B-9F33-8D3B6D0334FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Stafford, Erin E" &lt;estaffor@tulane.edu&gt;, </t>
   </si>
@@ -160,13 +160,28 @@
   </si>
   <si>
     <t xml:space="preserve">        diseases.</t>
+  </si>
+  <si>
+    <t>Away, but not forgotten</t>
+  </si>
+  <si>
+    <t>(Soodeh, Carrie, Ling, Kyle, Jessie, …. ) </t>
+  </si>
+  <si>
+    <t>www.linkedin.com/in/zhe-qu</t>
+  </si>
+  <si>
+    <t>PhD Candidate</t>
+  </si>
+  <si>
+    <t>I am a PhD candidate in Math Department of Tulane University. My current research interests are high dimensional data analysis, especially integrative analysis of neuroimaging or genomic data.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +211,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF212121"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -218,11 +240,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -538,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC129DD4-5708-4C25-BE56-42085CE9C315}">
-  <dimension ref="B1:J14"/>
+  <dimension ref="B1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C2:C14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +577,7 @@
     <col min="2" max="2" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>26</v>
       </c>
@@ -575,7 +603,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,7 +611,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -591,7 +619,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -599,7 +627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -610,7 +638,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -618,7 +646,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -626,7 +654,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -634,7 +662,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -656,67 +684,87 @@
       <c r="J9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="K9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N9" t="s">
+        <v>43</v>
+      </c>
+      <c r="O9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="J10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="J11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="J12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>
       </c>
-      <c r="J13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
       </c>
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="J14" t="s">
-        <v>44</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G9" r:id="rId1" xr:uid="{E7920C75-54EA-40FE-A984-9D0DD45CD352}"/>
+    <hyperlink ref="F14" r:id="rId2" display="http://www.linkedin.com/in/zhe-qu" xr:uid="{1354B411-9D63-4FA1-8781-C4A142645949}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added meta tags for SEO.
</commit_message>
<xml_diff>
--- a/People spreadsheet.xlsx
+++ b/People spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerrit\Documents\College BAAAAAYBEEEEEE\Math Bio Site\hymanlab.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1178E035-1D47-4868-A81C-F535494F6803}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DD50A3-76F6-4480-97E7-B71BCF362901}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="5955" xr2:uid="{9C06E373-AECE-4E5B-9F33-8D3B6D0334FB}"/>
   </bookViews>
@@ -569,7 +569,7 @@
   <dimension ref="B1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Highlighted people who already have entries on spreadsheet.
</commit_message>
<xml_diff>
--- a/People spreadsheet.xlsx
+++ b/People spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerrit\Documents\College BAAAAAYBEEEEEE\Math Bio Site\hymanlab.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DD50A3-76F6-4480-97E7-B71BCF362901}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214238C0-2040-4186-9346-01259B7D03E2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="5955" xr2:uid="{9C06E373-AECE-4E5B-9F33-8D3B6D0334FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Stafford, Erin E" &lt;estaffor@tulane.edu&gt;, </t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t>I am a PhD candidate in Math Department of Tulane University. My current research interests are high dimensional data analysis, especially integrative analysis of neuroimaging or genomic data.</t>
+  </si>
+  <si>
+    <t>Jessica Conrad</t>
+  </si>
+  <si>
+    <t>jconrad4@tulane.edu</t>
+  </si>
+  <si>
+    <t>https://jessicarconrad.github.io/</t>
+  </si>
+  <si>
+    <t>Graduate Student</t>
   </si>
 </sst>
 </file>
@@ -219,12 +231,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -240,17 +258,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -569,7 +589,7 @@
   <dimension ref="B1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,19 +623,19 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -627,22 +647,22 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -662,49 +682,49 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -724,38 +744,52 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1" t="s">
+    <row r="14" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="6" t="s">
         <v>49</v>
       </c>
     </row>
+    <row r="15" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="19" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -763,8 +797,9 @@
   <hyperlinks>
     <hyperlink ref="G9" r:id="rId1" xr:uid="{E7920C75-54EA-40FE-A984-9D0DD45CD352}"/>
     <hyperlink ref="F14" r:id="rId2" display="http://www.linkedin.com/in/zhe-qu" xr:uid="{1354B411-9D63-4FA1-8781-C4A142645949}"/>
+    <hyperlink ref="C15" r:id="rId3" xr:uid="{7FF20E8B-0982-4404-A974-9F864537CF87}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Li Guan to spreadsheet.
</commit_message>
<xml_diff>
--- a/People spreadsheet.xlsx
+++ b/People spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerrit\Documents\College BAAAAAYBEEEEEE\Math Bio Site\hymanlab.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214238C0-2040-4186-9346-01259B7D03E2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F300CF-B955-4279-8C60-FB95536B18A6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="5955" xr2:uid="{9C06E373-AECE-4E5B-9F33-8D3B6D0334FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Stafford, Erin E" &lt;estaffor@tulane.edu&gt;, </t>
   </si>
@@ -187,13 +187,33 @@
   </si>
   <si>
     <t>Graduate Student</t>
+  </si>
+  <si>
+    <t>Graduate  Student</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/li-guan-113244162/</t>
+  </si>
+  <si>
+    <r>
+      <t>My current research interest focuses on mathematical models in epidemiology. In particular, I am interested in general vector-borne transmission models with variable infectiousness as a function of time since infection, with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF111111"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>probability distributions for the rate of disease progression and with variability in susceptibility to infections. I am also interested in parameter sensitivity analysis, identification and estimations by fitting models to data.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +250,18 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF111111"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF111111"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -258,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -271,6 +303,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -588,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC129DD4-5708-4C25-BE56-42085CE9C315}">
   <dimension ref="B1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,20 +699,29 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Wu Tong to people.
</commit_message>
<xml_diff>
--- a/People spreadsheet.xlsx
+++ b/People spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerrit\Documents\College BAAAAAYBEEEEEE\Math Bio Site\hymanlab.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F300CF-B955-4279-8C60-FB95536B18A6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B69F8AD-7452-428F-BB85-0CD82A3DC2F3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="5955" xr2:uid="{9C06E373-AECE-4E5B-9F33-8D3B6D0334FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Stafford, Erin E" &lt;estaffor@tulane.edu&gt;, </t>
   </si>
@@ -208,12 +208,18 @@
       <t>probability distributions for the rate of disease progression and with variability in susceptibility to infections. I am also interested in parameter sensitivity analysis, identification and estimations by fitting models to data.</t>
     </r>
   </si>
+  <si>
+    <t>My current research interests include data assimilation algorithms, numerical methods for time-dependent PDEs, hyperbolic conservation laws and numerical analysis. My current project is on data assimilation by combining the underlying time-dependent PDE model and interpolation from scattered spatial observations to improve future predictions.</t>
+  </si>
+  <si>
+    <t>Post-Doc</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +268,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -290,7 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -304,6 +316,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -622,7 +635,7 @@
   <dimension ref="B1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,12 +791,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="6" t="s">
         <v>23</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Created an our works section, commented it out until I have data for it.
</commit_message>
<xml_diff>
--- a/People spreadsheet.xlsx
+++ b/People spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerrit\Documents\College BAAAAAYBEEEEEE\Math Bio Site\hymanlab.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B69F8AD-7452-428F-BB85-0CD82A3DC2F3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118F2143-7CE0-41D8-9C0F-8D6A5EB2E8A1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="5955" xr2:uid="{9C06E373-AECE-4E5B-9F33-8D3B6D0334FB}"/>
   </bookViews>
@@ -634,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC129DD4-5708-4C25-BE56-42085CE9C315}">
   <dimension ref="B1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added google scholar link to dr. hyman's section.
</commit_message>
<xml_diff>
--- a/People spreadsheet.xlsx
+++ b/People spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerrit\Documents\College BAAAAAYBEEEEEE\Math Bio Site\hymanlab.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118F2143-7CE0-41D8-9C0F-8D6A5EB2E8A1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF9F497-67A5-4A8D-8881-ACFFED4D2ACF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="5955" xr2:uid="{9C06E373-AECE-4E5B-9F33-8D3B6D0334FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Stafford, Erin E" &lt;estaffor@tulane.edu&gt;, </t>
   </si>
@@ -214,12 +214,54 @@
   <si>
     <t>Post-Doc</t>
   </si>
+  <si>
+    <t>"Hickmann, Kyle Scott" hickmank@lanl.gov</t>
+  </si>
+  <si>
+    <t>"Justin.K.Davis@sdstate.edu" </t>
+  </si>
+  <si>
+    <t>Justin.K.Davis@sdstate.edu</t>
+  </si>
+  <si>
+    <t>hickmank@lanl.gov</t>
+  </si>
+  <si>
+    <t>"Manore, Carrie Anna" </t>
+  </si>
+  <si>
+    <t>cmanore@lanl.gov</t>
+  </si>
+  <si>
+    <t>Soodeh Azizi </t>
+  </si>
+  <si>
+    <t>soodeh.azizi@gmail.com</t>
+  </si>
+  <si>
+    <t>"Thongsripong, Panpim" </t>
+  </si>
+  <si>
+    <t>pthongsr@tulane.edu</t>
+  </si>
+  <si>
+    <t>"Conrad, Jessica" </t>
+  </si>
+  <si>
+    <t>jconrad4@lanl.gov</t>
+  </si>
+  <si>
+    <t>Elliot Hill</t>
+  </si>
+  <si>
+    <t>ehill3@tulane.edu</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +316,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF17394D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -302,7 +350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -317,6 +365,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -632,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC129DD4-5708-4C25-BE56-42085CE9C315}">
-  <dimension ref="B1:O20"/>
+  <dimension ref="B1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,6 +756,24 @@
       <c r="E5" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="J5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="6" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
@@ -712,7 +783,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" s="6" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
@@ -725,16 +796,16 @@
       <c r="F7" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="J7" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -756,24 +827,6 @@
       <c r="I9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="10" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
@@ -783,12 +836,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="6" t="s">
         <v>22</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -801,9 +857,6 @@
       <c r="E12" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="9" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="13" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
@@ -844,14 +897,70 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" s="14" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B16" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -859,8 +968,14 @@
     <hyperlink ref="G9" r:id="rId1" xr:uid="{E7920C75-54EA-40FE-A984-9D0DD45CD352}"/>
     <hyperlink ref="F14" r:id="rId2" display="http://www.linkedin.com/in/zhe-qu" xr:uid="{1354B411-9D63-4FA1-8781-C4A142645949}"/>
     <hyperlink ref="C15" r:id="rId3" xr:uid="{7FF20E8B-0982-4404-A974-9F864537CF87}"/>
+    <hyperlink ref="B22" r:id="rId4" display="mailto:hickmank@lanl.gov" xr:uid="{992BA6DA-E17B-4BA2-894D-0A8E419B4036}"/>
+    <hyperlink ref="B23" r:id="rId5" display="mailto:cmanore@lanl.gov" xr:uid="{BD418878-6693-4A0D-9F89-880348375B88}"/>
+    <hyperlink ref="B24" r:id="rId6" display="mailto:soodeh.azizi@gmail.com" xr:uid="{715A99A0-8FD5-466A-9EB4-55F8E4F79AB2}"/>
+    <hyperlink ref="B25" r:id="rId7" display="mailto:pthongsr@tulane.edu" xr:uid="{84AADDD4-8058-48EB-A5CC-FBB275DC37C9}"/>
+    <hyperlink ref="B26" r:id="rId8" display="mailto:jconrad4@lanl.gov" xr:uid="{26233C90-D230-4EC0-9874-42A04F4A92E4}"/>
+    <hyperlink ref="C16" r:id="rId9" xr:uid="{C8C4C440-3862-457B-9F00-D36270143D13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId4"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added panpim to former members.
</commit_message>
<xml_diff>
--- a/People spreadsheet.xlsx
+++ b/People spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerrit\Documents\College BAAAAAYBEEEEEE\Math Bio Site\hymanlab.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF9F497-67A5-4A8D-8881-ACFFED4D2ACF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DAB87F-48E8-492E-9648-D90486DC82AC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="5955" xr2:uid="{9C06E373-AECE-4E5B-9F33-8D3B6D0334FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Stafford, Erin E" &lt;estaffor@tulane.edu&gt;, </t>
   </si>
@@ -239,12 +239,6 @@
     <t>soodeh.azizi@gmail.com</t>
   </si>
   <si>
-    <t>"Thongsripong, Panpim" </t>
-  </si>
-  <si>
-    <t>pthongsr@tulane.edu</t>
-  </si>
-  <si>
     <t>"Conrad, Jessica" </t>
   </si>
   <si>
@@ -255,13 +249,34 @@
   </si>
   <si>
     <t>ehill3@tulane.edu</t>
+  </si>
+  <si>
+    <t>Panpim Throngsripong</t>
+  </si>
+  <si>
+    <t>tpanpim@gmail.com</t>
+  </si>
+  <si>
+    <t>Ph.D. Student</t>
+  </si>
+  <si>
+    <t>My research revolves around mosquitoes and mosquito-borne viruses. Even though my background is in the biology and ecology of disease transmission, I have always been interested in using mathematical tools to understand how diseases spread. Specifically, I am interested in using novel methods to quantify various disease transmission parameters with the hope to bridge biology with modeling. Currently, I hold a postdoctoral position in the Microbiology Department at the California Academy of Sciences. Other topics I’m currently working on include virus discovery, disease ecology, and education and public outreach.</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/thongsripong/</t>
+  </si>
+  <si>
+    <t>https://tpanpim.wordpress.com</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/thongsripong/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,6 +337,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212121"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -350,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -370,6 +391,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -687,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC129DD4-5708-4C25-BE56-42085CE9C315}">
   <dimension ref="B1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,23 +922,24 @@
     </row>
     <row r="16" spans="2:15" s="14" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B16" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>60</v>
       </c>
@@ -923,7 +947,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
         <v>59</v>
       </c>
@@ -931,7 +955,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
         <v>63</v>
       </c>
@@ -939,7 +963,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
         <v>65</v>
       </c>
@@ -947,20 +971,35 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
+    <row r="25" spans="2:10" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B25" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" s="6" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -971,11 +1010,14 @@
     <hyperlink ref="B22" r:id="rId4" display="mailto:hickmank@lanl.gov" xr:uid="{992BA6DA-E17B-4BA2-894D-0A8E419B4036}"/>
     <hyperlink ref="B23" r:id="rId5" display="mailto:cmanore@lanl.gov" xr:uid="{BD418878-6693-4A0D-9F89-880348375B88}"/>
     <hyperlink ref="B24" r:id="rId6" display="mailto:soodeh.azizi@gmail.com" xr:uid="{715A99A0-8FD5-466A-9EB4-55F8E4F79AB2}"/>
-    <hyperlink ref="B25" r:id="rId7" display="mailto:pthongsr@tulane.edu" xr:uid="{84AADDD4-8058-48EB-A5CC-FBB275DC37C9}"/>
-    <hyperlink ref="B26" r:id="rId8" display="mailto:jconrad4@lanl.gov" xr:uid="{26233C90-D230-4EC0-9874-42A04F4A92E4}"/>
-    <hyperlink ref="C16" r:id="rId9" xr:uid="{C8C4C440-3862-457B-9F00-D36270143D13}"/>
+    <hyperlink ref="B26" r:id="rId7" display="mailto:jconrad4@lanl.gov" xr:uid="{26233C90-D230-4EC0-9874-42A04F4A92E4}"/>
+    <hyperlink ref="C16" r:id="rId8" xr:uid="{C8C4C440-3862-457B-9F00-D36270143D13}"/>
+    <hyperlink ref="C25" r:id="rId9" xr:uid="{B928184E-082A-48A9-AB10-1F6B8F345AC1}"/>
+    <hyperlink ref="F25" r:id="rId10" xr:uid="{9CB5608F-5746-4852-AE78-347AEB7C9AE0}"/>
+    <hyperlink ref="G25" r:id="rId11" display="https://tpanpim.wordpress.com/" xr:uid="{34D2A698-24D9-49F8-B4B6-61F7B6DB85E5}"/>
+    <hyperlink ref="H25" r:id="rId12" xr:uid="{8CC79A90-29E0-4CA9-8AE5-A4D000C6D76F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId10"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added rhea to people spreadsheet.
</commit_message>
<xml_diff>
--- a/People spreadsheet.xlsx
+++ b/People spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerrit\Documents\College BAAAAAYBEEEEEE\Math Bio Site\hymanlab.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F30B451-21F1-4586-B884-E91D06A13A23}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52C5EF1-C812-47AC-A28C-0712132EFF27}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="5955" xr2:uid="{9C06E373-AECE-4E5B-9F33-8D3B6D0334FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Stafford, Erin E" &lt;estaffor@tulane.edu&gt;, </t>
   </si>
@@ -288,6 +288,15 @@
   </si>
   <si>
     <t>My current research under the supervision of both Dr. Hyman and Qu places emphasis on the use of mathematics and graph/network theory to understand stochastic processes such as the spread of epidemics. Specifically, we determine at what point an epidemic model such as an SI, SIR, and SIS becomes predictable. In other words, at what point does a deterministic model dictate the behavior of the epidemic? Other areas of research interest include using uncertainty quantification and parameter estimation for network modeling and fitting data.</t>
+  </si>
+  <si>
+    <t>Undergraduate</t>
+  </si>
+  <si>
+    <t>I am an undergraduate student at Tulane University pursuing a Bachelor of Science degree in Mathematics and Chemistry. My research interests include exploring the results that different network structures have in regards to SIR, SIS, and SI epidemic models. Specifically, the stochastic and deterministic stages that these epidemics can be broken down into to better understand their time-dependent spread through a population.</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/in/rhea-kataria-1362a8132 </t>
   </si>
 </sst>
 </file>
@@ -396,7 +405,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -420,6 +429,9 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -737,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC129DD4-5708-4C25-BE56-42085CE9C315}">
   <dimension ref="B1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,13 +800,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
@@ -906,14 +932,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
+    <row r="12" spans="2:15" s="14" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="14" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1063,8 +1089,9 @@
     <hyperlink ref="H25" r:id="rId12" xr:uid="{8CC79A90-29E0-4CA9-8AE5-A4D000C6D76F}"/>
     <hyperlink ref="C4" r:id="rId13" xr:uid="{C04CCAB3-35FE-47FD-B030-C1FEC3FBB058}"/>
     <hyperlink ref="F8" r:id="rId14" xr:uid="{0FD47756-C2C0-4C04-BE3C-7495A5BAEA48}"/>
+    <hyperlink ref="F4" r:id="rId15" display="http://www.linkedin.com/in/rhea-kataria-1362a8132" xr:uid="{0E1DCA15-C9A6-4737-B452-7FA9C37F0B1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId15"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Jeremy to people spreadsheet.
</commit_message>
<xml_diff>
--- a/People spreadsheet.xlsx
+++ b/People spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerrit\Documents\College BAAAAAYBEEEEEE\Math Bio Site\hymanlab.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52C5EF1-C812-47AC-A28C-0712132EFF27}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32724E1-6194-4FC2-BF73-09C44371A014}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="5955" xr2:uid="{9C06E373-AECE-4E5B-9F33-8D3B6D0334FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="91">
   <si>
     <t>Stafford, Erin E" &lt;estaffor@tulane.edu&gt;, </t>
   </si>
@@ -297,6 +297,18 @@
   </si>
   <si>
     <t>www.linkedin.com/in/rhea-kataria-1362a8132 </t>
+  </si>
+  <si>
+    <t>Jeremy Dewar</t>
+  </si>
+  <si>
+    <t>jdewar@tulane.edu</t>
+  </si>
+  <si>
+    <t>https://github.com/jdewar</t>
+  </si>
+  <si>
+    <t>http://math.tulane.edu/~jdewar/</t>
   </si>
 </sst>
 </file>
@@ -747,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC129DD4-5708-4C25-BE56-42085CE9C315}">
-  <dimension ref="B1:O26"/>
+  <dimension ref="B1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,6 +1084,27 @@
       <c r="C26" s="6" t="s">
         <v>67</v>
       </c>
+    </row>
+    <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added Ling Xue to People Spreadsheet
</commit_message>
<xml_diff>
--- a/People spreadsheet.xlsx
+++ b/People spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerrit\Documents\College BAAAAAYBEEEEEE\Math Bio Site\hymanlab.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32724E1-6194-4FC2-BF73-09C44371A014}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F36D497-64AA-462A-9175-402CF0D0873E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="5955" xr2:uid="{9C06E373-AECE-4E5B-9F33-8D3B6D0334FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="96">
   <si>
     <t>Stafford, Erin E" &lt;estaffor@tulane.edu&gt;, </t>
   </si>
@@ -310,12 +310,27 @@
   <si>
     <t>http://math.tulane.edu/~jdewar/</t>
   </si>
+  <si>
+    <t>Ling Xue</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=9GSPC4wAAAAJ&amp;hl=en&amp;oi=sra</t>
+  </si>
+  <si>
+    <t>http://homepage.hrbeu.edu.cn/web/xueling</t>
+  </si>
+  <si>
+    <t>Dr. Xue research focuses on creating and analyzing mathematical modelis for the spread of infectious diseases.  Her research ranges from mosquito-borne diseases, such as dengue fever, Zika, and chikungunya to the modeling the spread of the Ebola Virus disease. </t>
+  </si>
+  <si>
+    <t>lxue2@tulane.edu</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,6 +404,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF201F1E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -417,7 +438,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -444,6 +465,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -759,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC129DD4-5708-4C25-BE56-42085CE9C315}">
-  <dimension ref="B1:O27"/>
+  <dimension ref="B1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,129 +1024,152 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="2:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+    <row r="17" spans="2:10" s="14" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B17" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
+    <row r="21" spans="2:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
+    <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C22" s="17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+    <row r="24" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F24" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="J24" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="2:10" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B25" s="5" t="s">
+    <row r="26" spans="2:10" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B26" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C26" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E26" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F26" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G26" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H26" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="J25" s="16" t="s">
+      <c r="J26" s="16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="7" t="s">
+    <row r="27" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
+    <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6" t="s">
+      <c r="D28" s="6"/>
+      <c r="E28" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F28" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G28" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G9" r:id="rId1" xr:uid="{E7920C75-54EA-40FE-A984-9D0DD45CD352}"/>
     <hyperlink ref="F14" r:id="rId2" display="http://www.linkedin.com/in/zhe-qu" xr:uid="{1354B411-9D63-4FA1-8781-C4A142645949}"/>
     <hyperlink ref="C15" r:id="rId3" xr:uid="{7FF20E8B-0982-4404-A974-9F864537CF87}"/>
-    <hyperlink ref="B22" r:id="rId4" display="mailto:hickmank@lanl.gov" xr:uid="{992BA6DA-E17B-4BA2-894D-0A8E419B4036}"/>
-    <hyperlink ref="B23" r:id="rId5" display="mailto:cmanore@lanl.gov" xr:uid="{BD418878-6693-4A0D-9F89-880348375B88}"/>
-    <hyperlink ref="B24" r:id="rId6" display="mailto:soodeh.azizi@gmail.com" xr:uid="{715A99A0-8FD5-466A-9EB4-55F8E4F79AB2}"/>
-    <hyperlink ref="B26" r:id="rId7" display="mailto:jconrad4@lanl.gov" xr:uid="{26233C90-D230-4EC0-9874-42A04F4A92E4}"/>
+    <hyperlink ref="B23" r:id="rId4" display="mailto:hickmank@lanl.gov" xr:uid="{992BA6DA-E17B-4BA2-894D-0A8E419B4036}"/>
+    <hyperlink ref="B24" r:id="rId5" display="mailto:cmanore@lanl.gov" xr:uid="{BD418878-6693-4A0D-9F89-880348375B88}"/>
+    <hyperlink ref="B25" r:id="rId6" display="mailto:soodeh.azizi@gmail.com" xr:uid="{715A99A0-8FD5-466A-9EB4-55F8E4F79AB2}"/>
+    <hyperlink ref="B27" r:id="rId7" display="mailto:jconrad4@lanl.gov" xr:uid="{26233C90-D230-4EC0-9874-42A04F4A92E4}"/>
     <hyperlink ref="C16" r:id="rId8" xr:uid="{C8C4C440-3862-457B-9F00-D36270143D13}"/>
-    <hyperlink ref="C25" r:id="rId9" xr:uid="{B928184E-082A-48A9-AB10-1F6B8F345AC1}"/>
-    <hyperlink ref="F25" r:id="rId10" xr:uid="{9CB5608F-5746-4852-AE78-347AEB7C9AE0}"/>
-    <hyperlink ref="G25" r:id="rId11" display="https://tpanpim.wordpress.com/" xr:uid="{34D2A698-24D9-49F8-B4B6-61F7B6DB85E5}"/>
-    <hyperlink ref="H25" r:id="rId12" xr:uid="{8CC79A90-29E0-4CA9-8AE5-A4D000C6D76F}"/>
+    <hyperlink ref="C26" r:id="rId9" xr:uid="{B928184E-082A-48A9-AB10-1F6B8F345AC1}"/>
+    <hyperlink ref="F26" r:id="rId10" xr:uid="{9CB5608F-5746-4852-AE78-347AEB7C9AE0}"/>
+    <hyperlink ref="G26" r:id="rId11" display="https://tpanpim.wordpress.com/" xr:uid="{34D2A698-24D9-49F8-B4B6-61F7B6DB85E5}"/>
+    <hyperlink ref="H26" r:id="rId12" xr:uid="{8CC79A90-29E0-4CA9-8AE5-A4D000C6D76F}"/>
     <hyperlink ref="C4" r:id="rId13" xr:uid="{C04CCAB3-35FE-47FD-B030-C1FEC3FBB058}"/>
     <hyperlink ref="F8" r:id="rId14" xr:uid="{0FD47756-C2C0-4C04-BE3C-7495A5BAEA48}"/>
     <hyperlink ref="F4" r:id="rId15" display="http://www.linkedin.com/in/rhea-kataria-1362a8132" xr:uid="{0E1DCA15-C9A6-4737-B452-7FA9C37F0B1E}"/>
+    <hyperlink ref="F17" r:id="rId16" tooltip="Original URL: https://scholar.google.com/citations?user=9GSPC4wAAAAJ&amp;hl=en&amp;oi=sra. Click or tap if you trust this link." display="https://nam03.safelinks.protection.outlook.com/?url=https%3A%2F%2Fscholar.google.com%2Fcitations%3Fuser%3D9GSPC4wAAAAJ%26hl%3Den%26oi%3Dsra&amp;data=02%7C01%7Cgvanbeek%40tulane.edu%7C743bfd7459c4434569c508d83f27f18a%7C9de9818325d94b139fc34de5489c1f3b%7C1%7C0%7C637328788073855812&amp;sdata=gI9mqIwO8ezahCzrfJ4TFRO7ABO0ggXSSEVCYwIDDBY%3D&amp;reserved=0" xr:uid="{9FF091D1-6E23-4C32-B474-E0CAF13D68CD}"/>
+    <hyperlink ref="G17" r:id="rId17" tooltip="Original URL: http://homepage.hrbeu.edu.cn/web/xueling. Click or tap if you trust this link." display="https://nam03.safelinks.protection.outlook.com/?url=http%3A%2F%2Fhomepage.hrbeu.edu.cn%2Fweb%2Fxueling&amp;data=02%7C01%7Cgvanbeek%40tulane.edu%7C743bfd7459c4434569c508d83f27f18a%7C9de9818325d94b139fc34de5489c1f3b%7C1%7C0%7C637328788073855812&amp;sdata=r%2F65rlw376QrX%2BwdLR4tcwk6dSDb9scoMpSoA5DRJS4%3D&amp;reserved=0" xr:uid="{EA248A8B-DA71-4FF3-A62A-6572E3BC1F1C}"/>
+    <hyperlink ref="C17" r:id="rId18" xr:uid="{68964F5F-C4E7-4C4E-BEE3-7D7D7E0777A9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId16"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Ling Xue to contact.html
</commit_message>
<xml_diff>
--- a/People spreadsheet.xlsx
+++ b/People spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerrit\Documents\College BAAAAAYBEEEEEE\Math Bio Site\hymanlab.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F36D497-64AA-462A-9175-402CF0D0873E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9694419-8637-4DCD-915C-5FEF5C33EDD0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="5955" xr2:uid="{9C06E373-AECE-4E5B-9F33-8D3B6D0334FB}"/>
   </bookViews>
@@ -465,7 +465,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -784,7 +784,7 @@
   <dimension ref="B1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B17" sqref="B17:O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,38 +1024,46 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="2:10" s="14" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B17" s="12" t="s">
+    <row r="17" spans="2:15" s="14" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B17" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="15" t="s">
         <v>95</v>
       </c>
+      <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="7" t="s">
         <v>93</v>
       </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
       <c r="J17" s="20" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="2:15" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>60</v>
       </c>
@@ -1063,7 +1071,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
         <v>59</v>
       </c>
@@ -1071,7 +1079,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
         <v>62</v>
       </c>
@@ -1088,7 +1096,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
         <v>64</v>
       </c>
@@ -1096,7 +1104,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="2:10" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
         <v>70</v>
       </c>
@@ -1119,7 +1127,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>66</v>
       </c>
@@ -1127,7 +1135,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
Updates zhuolin in people spreadsheet.
</commit_message>
<xml_diff>
--- a/People spreadsheet.xlsx
+++ b/People spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerrit\Documents\College BAAAAAYBEEEEEE\Math Bio Site\hymanlab.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9694419-8637-4DCD-915C-5FEF5C33EDD0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D97983-5B72-4CD3-8C79-1A6D626538DF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="5955" xr2:uid="{9C06E373-AECE-4E5B-9F33-8D3B6D0334FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
   <si>
     <t>Stafford, Erin E" &lt;estaffor@tulane.edu&gt;, </t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>rkataria@tulane.edu</t>
-  </si>
-  <si>
-    <t>zqu1@tulane.edu</t>
   </si>
   <si>
     <t>ylu6@tulane.edu</t>
@@ -324,6 +321,12 @@
   </si>
   <si>
     <t>lxue2@tulane.edu</t>
+  </si>
+  <si>
+    <t>zhuolin.qu@utsa.edu</t>
+  </si>
+  <si>
+    <t>Assistant Professor at UT San Antonio</t>
   </si>
 </sst>
 </file>
@@ -781,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC129DD4-5708-4C25-BE56-42085CE9C315}">
-  <dimension ref="B1:O28"/>
+  <dimension ref="B1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:O17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,28 +797,28 @@
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -843,341 +846,362 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
+    <row r="5" spans="2:15" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" s="6" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>56</v>
+      <c r="E7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="J8" s="18" t="s">
-        <v>83</v>
+      <c r="F8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="10" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="J10" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" s="14" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="E11" s="14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="2:15" s="14" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B12" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="14" t="s">
+    <row r="12" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="13" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="E13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="14" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>25</v>
+        <v>49</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>52</v>
+    </row>
+    <row r="15" spans="2:15" s="14" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B15" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="2:15" s="14" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B16" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="13" t="s">
+      <c r="B16" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+    </row>
+    <row r="17" spans="2:18" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:18" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B25" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="17" spans="2:15" s="14" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B17" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-    </row>
-    <row r="18" spans="2:15" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="C25" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="26" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B26" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="H26" s="7" t="s">
+      <c r="C26" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J26" s="16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="2:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="9" t="s">
+      <c r="F27" s="6" t="s">
         <v>88</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+    </row>
+    <row r="28" spans="2:18" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>90</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
+      <c r="J28" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+    </row>
+    <row r="29" spans="2:18" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B29" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G9" r:id="rId1" xr:uid="{E7920C75-54EA-40FE-A984-9D0DD45CD352}"/>
-    <hyperlink ref="F14" r:id="rId2" display="http://www.linkedin.com/in/zhe-qu" xr:uid="{1354B411-9D63-4FA1-8781-C4A142645949}"/>
-    <hyperlink ref="C15" r:id="rId3" xr:uid="{7FF20E8B-0982-4404-A974-9F864537CF87}"/>
-    <hyperlink ref="B23" r:id="rId4" display="mailto:hickmank@lanl.gov" xr:uid="{992BA6DA-E17B-4BA2-894D-0A8E419B4036}"/>
-    <hyperlink ref="B24" r:id="rId5" display="mailto:cmanore@lanl.gov" xr:uid="{BD418878-6693-4A0D-9F89-880348375B88}"/>
-    <hyperlink ref="B25" r:id="rId6" display="mailto:soodeh.azizi@gmail.com" xr:uid="{715A99A0-8FD5-466A-9EB4-55F8E4F79AB2}"/>
-    <hyperlink ref="B27" r:id="rId7" display="mailto:jconrad4@lanl.gov" xr:uid="{26233C90-D230-4EC0-9874-42A04F4A92E4}"/>
-    <hyperlink ref="C16" r:id="rId8" xr:uid="{C8C4C440-3862-457B-9F00-D36270143D13}"/>
-    <hyperlink ref="C26" r:id="rId9" xr:uid="{B928184E-082A-48A9-AB10-1F6B8F345AC1}"/>
-    <hyperlink ref="F26" r:id="rId10" xr:uid="{9CB5608F-5746-4852-AE78-347AEB7C9AE0}"/>
-    <hyperlink ref="G26" r:id="rId11" display="https://tpanpim.wordpress.com/" xr:uid="{34D2A698-24D9-49F8-B4B6-61F7B6DB85E5}"/>
-    <hyperlink ref="H26" r:id="rId12" xr:uid="{8CC79A90-29E0-4CA9-8AE5-A4D000C6D76F}"/>
+    <hyperlink ref="G8" r:id="rId1" xr:uid="{E7920C75-54EA-40FE-A984-9D0DD45CD352}"/>
+    <hyperlink ref="F13" r:id="rId2" display="http://www.linkedin.com/in/zhe-qu" xr:uid="{1354B411-9D63-4FA1-8781-C4A142645949}"/>
+    <hyperlink ref="C14" r:id="rId3" xr:uid="{7FF20E8B-0982-4404-A974-9F864537CF87}"/>
+    <hyperlink ref="B22" r:id="rId4" display="mailto:hickmank@lanl.gov" xr:uid="{992BA6DA-E17B-4BA2-894D-0A8E419B4036}"/>
+    <hyperlink ref="B23" r:id="rId5" display="mailto:cmanore@lanl.gov" xr:uid="{BD418878-6693-4A0D-9F89-880348375B88}"/>
+    <hyperlink ref="B24" r:id="rId6" display="mailto:soodeh.azizi@gmail.com" xr:uid="{715A99A0-8FD5-466A-9EB4-55F8E4F79AB2}"/>
+    <hyperlink ref="B26" r:id="rId7" display="mailto:jconrad4@lanl.gov" xr:uid="{26233C90-D230-4EC0-9874-42A04F4A92E4}"/>
+    <hyperlink ref="C15" r:id="rId8" xr:uid="{C8C4C440-3862-457B-9F00-D36270143D13}"/>
+    <hyperlink ref="C25" r:id="rId9" xr:uid="{B928184E-082A-48A9-AB10-1F6B8F345AC1}"/>
+    <hyperlink ref="F25" r:id="rId10" xr:uid="{9CB5608F-5746-4852-AE78-347AEB7C9AE0}"/>
+    <hyperlink ref="G25" r:id="rId11" display="https://tpanpim.wordpress.com/" xr:uid="{34D2A698-24D9-49F8-B4B6-61F7B6DB85E5}"/>
+    <hyperlink ref="H25" r:id="rId12" xr:uid="{8CC79A90-29E0-4CA9-8AE5-A4D000C6D76F}"/>
     <hyperlink ref="C4" r:id="rId13" xr:uid="{C04CCAB3-35FE-47FD-B030-C1FEC3FBB058}"/>
-    <hyperlink ref="F8" r:id="rId14" xr:uid="{0FD47756-C2C0-4C04-BE3C-7495A5BAEA48}"/>
+    <hyperlink ref="F7" r:id="rId14" xr:uid="{0FD47756-C2C0-4C04-BE3C-7495A5BAEA48}"/>
     <hyperlink ref="F4" r:id="rId15" display="http://www.linkedin.com/in/rhea-kataria-1362a8132" xr:uid="{0E1DCA15-C9A6-4737-B452-7FA9C37F0B1E}"/>
-    <hyperlink ref="F17" r:id="rId16" tooltip="Original URL: https://scholar.google.com/citations?user=9GSPC4wAAAAJ&amp;hl=en&amp;oi=sra. Click or tap if you trust this link." display="https://nam03.safelinks.protection.outlook.com/?url=https%3A%2F%2Fscholar.google.com%2Fcitations%3Fuser%3D9GSPC4wAAAAJ%26hl%3Den%26oi%3Dsra&amp;data=02%7C01%7Cgvanbeek%40tulane.edu%7C743bfd7459c4434569c508d83f27f18a%7C9de9818325d94b139fc34de5489c1f3b%7C1%7C0%7C637328788073855812&amp;sdata=gI9mqIwO8ezahCzrfJ4TFRO7ABO0ggXSSEVCYwIDDBY%3D&amp;reserved=0" xr:uid="{9FF091D1-6E23-4C32-B474-E0CAF13D68CD}"/>
-    <hyperlink ref="G17" r:id="rId17" tooltip="Original URL: http://homepage.hrbeu.edu.cn/web/xueling. Click or tap if you trust this link." display="https://nam03.safelinks.protection.outlook.com/?url=http%3A%2F%2Fhomepage.hrbeu.edu.cn%2Fweb%2Fxueling&amp;data=02%7C01%7Cgvanbeek%40tulane.edu%7C743bfd7459c4434569c508d83f27f18a%7C9de9818325d94b139fc34de5489c1f3b%7C1%7C0%7C637328788073855812&amp;sdata=r%2F65rlw376QrX%2BwdLR4tcwk6dSDb9scoMpSoA5DRJS4%3D&amp;reserved=0" xr:uid="{EA248A8B-DA71-4FF3-A62A-6572E3BC1F1C}"/>
-    <hyperlink ref="C17" r:id="rId18" xr:uid="{68964F5F-C4E7-4C4E-BEE3-7D7D7E0777A9}"/>
+    <hyperlink ref="F16" r:id="rId16" tooltip="Original URL: https://scholar.google.com/citations?user=9GSPC4wAAAAJ&amp;hl=en&amp;oi=sra. Click or tap if you trust this link." display="https://nam03.safelinks.protection.outlook.com/?url=https%3A%2F%2Fscholar.google.com%2Fcitations%3Fuser%3D9GSPC4wAAAAJ%26hl%3Den%26oi%3Dsra&amp;data=02%7C01%7Cgvanbeek%40tulane.edu%7C743bfd7459c4434569c508d83f27f18a%7C9de9818325d94b139fc34de5489c1f3b%7C1%7C0%7C637328788073855812&amp;sdata=gI9mqIwO8ezahCzrfJ4TFRO7ABO0ggXSSEVCYwIDDBY%3D&amp;reserved=0" xr:uid="{9FF091D1-6E23-4C32-B474-E0CAF13D68CD}"/>
+    <hyperlink ref="G16" r:id="rId17" tooltip="Original URL: http://homepage.hrbeu.edu.cn/web/xueling. Click or tap if you trust this link." display="https://nam03.safelinks.protection.outlook.com/?url=http%3A%2F%2Fhomepage.hrbeu.edu.cn%2Fweb%2Fxueling&amp;data=02%7C01%7Cgvanbeek%40tulane.edu%7C743bfd7459c4434569c508d83f27f18a%7C9de9818325d94b139fc34de5489c1f3b%7C1%7C0%7C637328788073855812&amp;sdata=r%2F65rlw376QrX%2BwdLR4tcwk6dSDb9scoMpSoA5DRJS4%3D&amp;reserved=0" xr:uid="{EA248A8B-DA71-4FF3-A62A-6572E3BC1F1C}"/>
+    <hyperlink ref="C16" r:id="rId18" xr:uid="{68964F5F-C4E7-4C4E-BEE3-7D7D7E0777A9}"/>
+    <hyperlink ref="C29" r:id="rId19" xr:uid="{1785685F-B0CB-4A1D-8894-6311D465368F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId19"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Emily Meyer's information in the people spreadsheet.
</commit_message>
<xml_diff>
--- a/People spreadsheet.xlsx
+++ b/People spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerrit\Documents\College BAAAAAYBEEEEEE\Math Bio Site\hymanlab.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D97983-5B72-4CD3-8C79-1A6D626538DF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA830005-155A-4805-ABAF-29A11F7D393E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="5955" xr2:uid="{9C06E373-AECE-4E5B-9F33-8D3B6D0334FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="100">
   <si>
     <t>Stafford, Erin E" &lt;estaffor@tulane.edu&gt;, </t>
   </si>
@@ -327,6 +327,15 @@
   </si>
   <si>
     <t>Assistant Professor at UT San Antonio</t>
+  </si>
+  <si>
+    <t>Post Bac Researcher</t>
+  </si>
+  <si>
+    <t>I am a postbac fellow at the National Institutes of Health. I am interested in visual neuroscience, specifically comparing behavior with higher-level processing through experimental and computational methods. I graduated Tulane in 2019 with majors in mathematics and neuroscience and a public health minor. With the Mathematical Modeling and Analysis Lab, I studied the effects of diabetes on the progression and drug resistance of tuberculosis. I also previously worked on modeling vector-borne diseases with multiple risk groups and behavioral factors.</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/emily-meyer-769a95158/</t>
   </si>
 </sst>
 </file>
@@ -784,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC129DD4-5708-4C25-BE56-42085CE9C315}">
-  <dimension ref="B1:R29"/>
+  <dimension ref="B1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,14 +838,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
+    <row r="3" spans="2:15" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>2</v>
@@ -1178,6 +1180,28 @@
       <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
+    </row>
+    <row r="30" spans="2:18" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="K30" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1200,8 +1224,9 @@
     <hyperlink ref="G16" r:id="rId17" tooltip="Original URL: http://homepage.hrbeu.edu.cn/web/xueling. Click or tap if you trust this link." display="https://nam03.safelinks.protection.outlook.com/?url=http%3A%2F%2Fhomepage.hrbeu.edu.cn%2Fweb%2Fxueling&amp;data=02%7C01%7Cgvanbeek%40tulane.edu%7C743bfd7459c4434569c508d83f27f18a%7C9de9818325d94b139fc34de5489c1f3b%7C1%7C0%7C637328788073855812&amp;sdata=r%2F65rlw376QrX%2BwdLR4tcwk6dSDb9scoMpSoA5DRJS4%3D&amp;reserved=0" xr:uid="{EA248A8B-DA71-4FF3-A62A-6572E3BC1F1C}"/>
     <hyperlink ref="C16" r:id="rId18" xr:uid="{68964F5F-C4E7-4C4E-BEE3-7D7D7E0777A9}"/>
     <hyperlink ref="C29" r:id="rId19" xr:uid="{1785685F-B0CB-4A1D-8894-6311D465368F}"/>
+    <hyperlink ref="F30" r:id="rId20" xr:uid="{7A39FB7B-EB75-468F-B223-C0C09F75D15F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId20"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Emily Meyers contact email.
</commit_message>
<xml_diff>
--- a/People spreadsheet.xlsx
+++ b/People spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerrit\Documents\College BAAAAAYBEEEEEE\Math Bio Site\hymanlab.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA830005-155A-4805-ABAF-29A11F7D393E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EE0EC0-FE0E-4B3C-AA3A-8B0D8CE81EA0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="5955" xr2:uid="{9C06E373-AECE-4E5B-9F33-8D3B6D0334FB}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t>estaffor@tulane.edu</t>
   </si>
   <si>
-    <t>emeyer2@tulane.edu</t>
-  </si>
-  <si>
     <t>rkataria@tulane.edu</t>
   </si>
   <si>
@@ -336,6 +333,9 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/emily-meyer-769a95158/</t>
+  </si>
+  <si>
+    <t>emeyer121@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -796,7 +796,7 @@
   <dimension ref="B1:R30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:K30"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,28 +806,28 @@
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -844,20 +844,20 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K4" s="6"/>
     </row>
@@ -867,7 +867,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -875,16 +875,16 @@
         <v>6</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="J7" s="18" t="s">
         <v>81</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="8" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -892,19 +892,19 @@
         <v>7</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="H8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -912,7 +912,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -920,10 +920,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="2:15" s="14" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -931,10 +931,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -942,7 +942,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -950,61 +950,61 @@
         <v>12</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="14" spans="2:15" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="E14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="15" spans="2:15" s="14" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="16" spans="2:15" s="14" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
@@ -1015,102 +1015,102 @@
     <row r="17" spans="2:18" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:18" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="2:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>62</v>
-      </c>
       <c r="E23" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J23" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
         <v>63</v>
-      </c>
-      <c r="C24" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="25" spans="2:18" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="E25" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="F25" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J25" s="16" t="s">
         <v>71</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="26" spans="2:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="27" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>87</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F27" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>89</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
@@ -1121,20 +1121,20 @@
         <v>5</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>54</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
       <c r="J28" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
@@ -1149,33 +1149,33 @@
         <v>3</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K29" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K29" s="6" t="s">
+      <c r="L29" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="L29" s="6" t="s">
+      <c r="M29" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M29" s="6" t="s">
+      <c r="N29" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="N29" s="6" t="s">
+      <c r="O29" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="O29" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
@@ -1185,21 +1185,21 @@
       <c r="B30" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>14</v>
+      <c r="C30" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K30" s="6"/>
     </row>
@@ -1225,8 +1225,9 @@
     <hyperlink ref="C16" r:id="rId18" xr:uid="{68964F5F-C4E7-4C4E-BEE3-7D7D7E0777A9}"/>
     <hyperlink ref="C29" r:id="rId19" xr:uid="{1785685F-B0CB-4A1D-8894-6311D465368F}"/>
     <hyperlink ref="F30" r:id="rId20" xr:uid="{7A39FB7B-EB75-468F-B223-C0C09F75D15F}"/>
+    <hyperlink ref="C30" r:id="rId21" display="mailto:emeyer121@gmail.com" xr:uid="{0DCDC9C7-37F3-4AFA-BB68-CAE5FBE79151}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId21"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>